<commit_message>
Inbox data laboproef aangevuld op 04/06/18
</commit_message>
<xml_diff>
--- a/data/inbox/Logger_record_overzicht.xlsx
+++ b/data/inbox/Logger_record_overzicht.xlsx
@@ -198,20 +198,11 @@
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -220,6 +211,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -524,7 +524,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,197 +535,209 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>43243</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="10">
         <v>4171</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>5083</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="10">
         <v>5082</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>4148</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="12">
         <v>4148</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="15"/>
+      <c r="A4" s="4">
+        <v>43255</v>
+      </c>
+      <c r="B4" s="10">
+        <v>4435</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5370</v>
+      </c>
+      <c r="D4" s="10">
+        <v>5369</v>
+      </c>
+      <c r="E4" s="3">
+        <v>4435</v>
+      </c>
+      <c r="F4" s="12">
+        <v>4435</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="15"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="15"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="15"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="15"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="15"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="15"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="15"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="15"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="15"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="15"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="15"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="15"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="15"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="15"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="15"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="15"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="16"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>